<commit_message>
Added some new Picture from TC and TD
</commit_message>
<xml_diff>
--- a/Bilder.xlsx
+++ b/Bilder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/myzinsky/Programming/HamExamImages/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551DE5E8-1C4E-2F43-A28E-0AA59297C72F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC600B6-4899-CF41-A586-CA5F5819ACA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{61BD45D1-9088-114A-9BE1-3E0548C49E30}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="246">
   <si>
     <t>TC525</t>
   </si>
@@ -718,6 +718,51 @@
   </si>
   <si>
     <t>TC709</t>
+  </si>
+  <si>
+    <t>TD226-4</t>
+  </si>
+  <si>
+    <t>TD226-3</t>
+  </si>
+  <si>
+    <t>TD226-2</t>
+  </si>
+  <si>
+    <t>TD226-1</t>
+  </si>
+  <si>
+    <t>TD120</t>
+  </si>
+  <si>
+    <t>TD229</t>
+  </si>
+  <si>
+    <t>TD230</t>
+  </si>
+  <si>
+    <t>TC301-2</t>
+  </si>
+  <si>
+    <t>TC301-1</t>
+  </si>
+  <si>
+    <t>TC301-4</t>
+  </si>
+  <si>
+    <t>TC301-3</t>
+  </si>
+  <si>
+    <t>TC202-1</t>
+  </si>
+  <si>
+    <t>TC202-2</t>
+  </si>
+  <si>
+    <t>TC202-3</t>
+  </si>
+  <si>
+    <t>TC202-4</t>
   </si>
 </sst>
 </file>
@@ -1124,8 +1169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9246B77-698D-CD41-8067-E8817BC12991}">
   <dimension ref="A1:H225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="D122" sqref="D122"/>
+    <sheetView tabSelected="1" topLeftCell="A140" zoomScale="98" workbookViewId="0">
+      <selection activeCell="F159" sqref="F159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1176,7 +1221,7 @@
       </c>
       <c r="H3">
         <f>COUNTA(B:E)</f>
-        <v>229</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1194,7 +1239,7 @@
       </c>
       <c r="H4">
         <f>COUNTA(B:B)</f>
-        <v>164</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1231,7 +1276,7 @@
       </c>
       <c r="H7">
         <f>H3+16</f>
-        <v>245</v>
+        <v>260</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -2456,7 +2501,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" s="2">
         <v>156</v>
       </c>
@@ -2467,7 +2512,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" s="2">
         <v>157</v>
       </c>
@@ -2475,7 +2520,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" s="2">
         <v>158</v>
       </c>
@@ -2483,7 +2528,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" s="2">
         <v>159</v>
       </c>
@@ -2491,7 +2536,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" s="2">
         <v>160</v>
       </c>
@@ -2499,7 +2544,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" s="2">
         <v>161</v>
       </c>
@@ -2510,7 +2555,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" s="2">
         <v>162</v>
       </c>
@@ -2518,7 +2563,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" s="2">
         <v>163</v>
       </c>
@@ -2526,7 +2571,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" s="2">
         <v>164</v>
       </c>
@@ -2534,7 +2579,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" s="2">
         <v>165</v>
       </c>
@@ -2544,8 +2589,11 @@
       <c r="C154" s="3" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D154" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" s="2">
         <v>166</v>
       </c>
@@ -2556,7 +2604,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" s="2">
         <v>167</v>
       </c>
@@ -2566,8 +2614,11 @@
       <c r="C156" s="3" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D156" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" s="2">
         <v>168</v>
       </c>
@@ -2578,7 +2629,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" s="2">
         <v>169</v>
       </c>
@@ -2586,7 +2637,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" s="2">
         <v>170</v>
       </c>
@@ -2594,7 +2645,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" s="2">
         <v>171</v>
       </c>
@@ -2609,6 +2660,9 @@
       <c r="B161" s="3" t="s">
         <v>215</v>
       </c>
+      <c r="C161" s="3" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" s="2">
@@ -2698,108 +2752,144 @@
       <c r="A171" s="2">
         <v>182</v>
       </c>
+      <c r="B171" s="3" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" s="2">
         <v>183</v>
       </c>
+      <c r="B172" s="3" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" s="2">
         <v>184</v>
       </c>
+      <c r="B173" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" s="2">
         <v>185</v>
       </c>
+      <c r="B174" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="C174" s="3" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" s="2">
         <v>186</v>
       </c>
+      <c r="B175" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" s="2">
         <v>187</v>
       </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B176" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" s="2">
         <v>188</v>
       </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B177" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" s="2">
         <v>189</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" s="2">
         <v>190</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" s="2">
         <v>191</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" s="2">
         <v>192</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182" s="2">
         <v>193</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183" s="2">
         <v>194</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184" s="2">
         <v>195</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A185" s="2">
         <v>196</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186" s="2">
         <v>197</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187" s="2">
         <v>198</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188" s="2">
         <v>199</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189" s="2">
         <v>200</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190" s="2">
         <v>201</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191" s="2">
         <v>202</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192" s="2">
         <v>203</v>
       </c>

</xml_diff>

<commit_message>
Added TD201 and TD202
</commit_message>
<xml_diff>
--- a/Bilder.xlsx
+++ b/Bilder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/myzinsky/Programming/HamExamImages/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC600B6-4899-CF41-A586-CA5F5819ACA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4A39C0-74AE-0C43-945C-B58C2A9953B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{61BD45D1-9088-114A-9BE1-3E0548C49E30}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16520" xr2:uid="{61BD45D1-9088-114A-9BE1-3E0548C49E30}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="248">
   <si>
     <t>TC525</t>
   </si>
@@ -763,13 +763,19 @@
   </si>
   <si>
     <t>TC202-4</t>
+  </si>
+  <si>
+    <t>TD201</t>
+  </si>
+  <si>
+    <t>TD202</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -788,6 +794,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -846,13 +859,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1169,8 +1183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9246B77-698D-CD41-8067-E8817BC12991}">
   <dimension ref="A1:H225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A140" zoomScale="98" workbookViewId="0">
-      <selection activeCell="F159" sqref="F159"/>
+    <sheetView tabSelected="1" topLeftCell="A153" zoomScale="98" workbookViewId="0">
+      <selection activeCell="B179" sqref="B179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1188,7 +1202,7 @@
       <c r="B1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="6" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1221,7 +1235,7 @@
       </c>
       <c r="H3">
         <f>COUNTA(B:E)</f>
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1239,7 +1253,7 @@
       </c>
       <c r="H4">
         <f>COUNTA(B:B)</f>
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1274,10 +1288,6 @@
       <c r="C7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H7">
-        <f>H3+16</f>
-        <v>260</v>
-      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
@@ -2823,10 +2833,16 @@
       <c r="A178" s="2">
         <v>189</v>
       </c>
+      <c r="B178" s="3" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" s="2">
         <v>190</v>
+      </c>
+      <c r="B179" s="3" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>